<commit_message>
Final update semester planning
</commit_message>
<xml_diff>
--- a/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
+++ b/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Arbeitspacket</t>
   </si>
@@ -129,13 +129,58 @@
   </si>
   <si>
     <t>"How To" zum Laden von XML in Unity</t>
+  </si>
+  <si>
+    <t>Meilenstein 5 (13.12.2017)</t>
+  </si>
+  <si>
+    <t>Überarbeiten der XML-Struktur für Steg</t>
+  </si>
+  <si>
+    <t>Erstellung interaktive Dokumentation</t>
+  </si>
+  <si>
+    <t>Tutorials erstellen</t>
+  </si>
+  <si>
+    <t>Testdaten interaktiv gestalten</t>
+  </si>
+  <si>
+    <t>Überarbeitung Tunnelgenerierung anhand XML</t>
+  </si>
+  <si>
+    <t>Endabgabe (22.12.2017)</t>
+  </si>
+  <si>
+    <t>Wissenschaftlicher Artikel erstellen</t>
+  </si>
+  <si>
+    <t>PMP fertigstellen</t>
+  </si>
+  <si>
+    <t>Systemdokumentation fertigstellen</t>
+  </si>
+  <si>
+    <t>Testdurchführung</t>
+  </si>
+  <si>
+    <t>Analyse Testdaten</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>SOLL</t>
+  </si>
+  <si>
+    <t>IST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +197,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,20 +249,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -524,24 +588,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:F27"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
-    <col min="2" max="2" width="48.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -568,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -596,7 +659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -624,7 +687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -652,7 +715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -680,26 +743,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4">
         <f>SUM(H2:H5)</f>
         <v>72</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f>SUM(I2:I5)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -727,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -755,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -783,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -811,7 +874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -839,26 +902,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4">
         <f>SUM(H7:H11)</f>
         <v>48</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <f>SUM(I7:I11)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -886,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -906,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:I27" si="4">C14+E14</f>
+        <f t="shared" ref="H14:I40" si="4">C14+E14</f>
         <v>8</v>
       </c>
       <c r="I14">
@@ -914,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -942,7 +1005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -970,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -998,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1026,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1054,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>80</v>
       </c>
@@ -1082,26 +1145,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4">
         <f>SUM(H13:H20)</f>
         <v>48</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <f>SUM(I13:I20)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1111,13 +1174,13 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22" s="6">
-        <v>4</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="D22" s="5">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
         <v>0</v>
       </c>
       <c r="H22">
@@ -1129,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1139,13 +1202,13 @@
       <c r="C23">
         <v>8</v>
       </c>
-      <c r="D23" s="6">
-        <v>8</v>
-      </c>
-      <c r="E23" s="6">
-        <v>4</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="D23" s="5">
+        <v>8</v>
+      </c>
+      <c r="E23" s="5">
+        <v>4</v>
+      </c>
+      <c r="F23" s="5">
         <v>2</v>
       </c>
       <c r="H23">
@@ -1157,7 +1220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1167,13 +1230,13 @@
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>16</v>
       </c>
-      <c r="E24" s="6">
-        <v>8</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="E24" s="5">
+        <v>8</v>
+      </c>
+      <c r="F24" s="5">
         <v>8</v>
       </c>
       <c r="H24">
@@ -1185,7 +1248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1195,13 +1258,13 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="6">
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
         <v>5</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>7</v>
       </c>
       <c r="H25">
@@ -1213,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1223,13 +1286,13 @@
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26" s="6">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6">
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
         <v>5</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>7</v>
       </c>
       <c r="H26">
@@ -1241,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1251,13 +1314,13 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27" s="6">
-        <v>0</v>
-      </c>
-      <c r="E27" s="6">
-        <v>4</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5">
         <v>4</v>
       </c>
       <c r="H27">
@@ -1269,31 +1332,405 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" s="5">
+        <v>8</v>
+      </c>
+      <c r="E28" s="5">
+        <v>8</v>
+      </c>
+      <c r="F28" s="5">
+        <v>8</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="5">
+        <v>6</v>
+      </c>
+      <c r="E29" s="5">
+        <v>4</v>
+      </c>
+      <c r="F29" s="5">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5">
-        <f>SUM(H22:H27)</f>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4">
+        <f>SUM(H22:H29)</f>
+        <v>72</v>
+      </c>
+      <c r="I30" s="4">
+        <f>SUM(I22:I29)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>8</v>
+      </c>
+      <c r="F31" s="7">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" s="7">
+        <v>14</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" s="5">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" s="5">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35" s="7">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="4">
+        <f>SUM(H31:H35)</f>
         <v>48</v>
       </c>
-      <c r="I28" s="5">
-        <f>SUM(I22:I27)</f>
+      <c r="I36" s="4">
+        <f>SUM(I31:I35)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" s="7">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37" s="7">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38" s="7">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39" s="7">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" s="7">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="4">
+        <f>SUM(H37:H40)</f>
+        <v>48</v>
+      </c>
+      <c r="I41" s="4">
+        <f>SUM(I37:I40)</f>
         <v>56</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8">
+        <f>H41+H36+H30+H21+H12+H6</f>
+        <v>336</v>
+      </c>
+      <c r="I44" s="8">
+        <f>I41+I36+I30+I21+I12+I6</f>
+        <v>370</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B28:F28"/>
+  <mergeCells count="6">
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B30:F30"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B36:F36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
journal & planning documents
</commit_message>
<xml_diff>
--- a/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
+++ b/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DummyUser\Documents\Vortex\pawi-vortext-tunnel\01_Dokumentation\01_Rahmenplanung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tagroebe\Documents\Term_5\PAWI\pawi-vortex-tunnel-newest\01_Dokumentation\01_Rahmenplanung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,12 +155,6 @@
     <t>Wissenschaftlicher Artikel erstellen</t>
   </si>
   <si>
-    <t>PMP fertigstellen</t>
-  </si>
-  <si>
-    <t>Systemdokumentation fertigstellen</t>
-  </si>
-  <si>
     <t>Testdurchführung</t>
   </si>
   <si>
@@ -174,12 +168,18 @@
   </si>
   <si>
     <t>IST</t>
+  </si>
+  <si>
+    <t>Systemdokumentation weiterführen</t>
+  </si>
+  <si>
+    <t>PMP weiterführen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,17 +269,45 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -590,21 +618,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -631,7 +659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -659,7 +687,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -687,7 +715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -715,7 +743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -743,15 +771,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4">
         <f>SUM(H2:H5)</f>
@@ -762,7 +790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -790,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -818,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -846,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -874,7 +902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -902,15 +930,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="3"/>
       <c r="H12" s="4">
         <f>SUM(H7:H11)</f>
@@ -921,7 +949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -949,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -977,7 +1005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1005,7 +1033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1033,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1061,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1089,7 +1117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1117,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>80</v>
       </c>
@@ -1145,15 +1173,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4">
         <f>SUM(H13:H20)</f>
@@ -1164,7 +1192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1192,7 +1220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1220,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1248,7 +1276,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1276,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1304,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1332,12 +1360,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -1360,12 +1388,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1388,15 +1416,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="3"/>
       <c r="H30" s="4">
         <f>SUM(H22:H29)</f>
@@ -1407,7 +1435,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1417,13 +1445,13 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31" s="7">
-        <v>0</v>
-      </c>
-      <c r="E31" s="7">
-        <v>8</v>
-      </c>
-      <c r="F31" s="7">
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <v>8</v>
+      </c>
+      <c r="F31" s="6">
         <v>8</v>
       </c>
       <c r="H31">
@@ -1435,7 +1463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1445,10 +1473,10 @@
       <c r="C32">
         <v>12</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>14</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
       <c r="F32" s="5">
@@ -1463,7 +1491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1473,7 +1501,7 @@
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>0</v>
       </c>
       <c r="E33">
@@ -1491,7 +1519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1501,7 +1529,7 @@
       <c r="C34">
         <v>0</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>0</v>
       </c>
       <c r="E34">
@@ -1519,7 +1547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1529,7 +1557,7 @@
       <c r="C35">
         <v>12</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>10</v>
       </c>
       <c r="E35">
@@ -1547,15 +1575,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4">
         <f>SUM(H31:H35)</f>
@@ -1566,7 +1594,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>28</v>
       </c>
@@ -1576,13 +1604,13 @@
       <c r="C37">
         <v>4</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>6</v>
       </c>
       <c r="E37">
         <v>4</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>6</v>
       </c>
       <c r="H37">
@@ -1594,17 +1622,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C38">
         <v>8</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>8</v>
       </c>
       <c r="E38">
@@ -1622,17 +1650,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C39">
         <v>8</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="6">
         <v>8</v>
       </c>
       <c r="E39">
@@ -1650,7 +1678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>31</v>
       </c>
@@ -1660,7 +1688,7 @@
       <c r="C40">
         <v>4</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>6</v>
       </c>
       <c r="E40">
@@ -1678,15 +1706,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
       <c r="G41" s="3"/>
       <c r="H41" s="4">
         <f>SUM(H37:H40)</f>
@@ -1697,28 +1725,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8">
+    </row>
+    <row r="44" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7">
         <f>H41+H36+H30+H21+H12+H6</f>
         <v>336</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="7">
         <f>I41+I36+I30+I21+I12+I6</f>
         <v>370</v>
       </c>

</xml_diff>

<commit_message>
Update all time used for handin
</commit_message>
<xml_diff>
--- a/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
+++ b/01_Dokumentation/01_Rahmenplanung/LaufendeRahmenplanung.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tagroebe\Documents\Term_5\PAWI\pawi-vortex-tunnel-newest\01_Dokumentation\01_Rahmenplanung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DummyUser\Documents\Vortex\pawi-vortext-tunnel\01_Dokumentation\01_Rahmenplanung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -179,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,21 +618,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,7 +659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -687,7 +687,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -715,7 +715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -743,7 +743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -771,7 +771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="8" t="s">
         <v>27</v>
@@ -790,7 +790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -818,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -846,7 +846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -874,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -902,7 +902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -930,7 +930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -949,7 +949,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>80</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -1192,7 +1192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="8" t="s">
         <v>49</v>
@@ -1435,7 +1435,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="8" t="s">
         <v>34</v>
@@ -1594,7 +1594,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>29</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>30</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>31</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="8" t="s">
         <v>40</v>
@@ -1725,7 +1725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
         <v>45</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="7" t="s">
         <v>44</v>
       </c>

</xml_diff>